<commit_message>
Progression, Menus and Lighting
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -102,7 +102,48 @@
     </r>
   </si>
   <si>
-    <t>Next Up: Moveable tile animation.</t>
+    <t>Tile movement is now animated!</t>
+  </si>
+  <si>
+    <t>Added pause/start menu foundations.</t>
+  </si>
+  <si>
+    <t>Added level progression.</t>
+  </si>
+  <si>
+    <t>Changed menu colors, added help menu (how to play) + localization, added keybinds to focus on player (Lshift) and reset grid panning (Tab). The "R" key now resets the current level rather than the entire game. Added new fonts! Added lighting!</t>
+  </si>
+  <si>
+    <r>
+      <t>Changed grid to naturally center on player. Pressing shift toggles focus. Tab only resets grid if non-centered. Fixed level change bug (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DISABLED LIGHTS TEMPORARILY, ROOT CAUSE NOT FOUND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>). Changed lightmask texture.</t>
+    </r>
+  </si>
+  <si>
+    <t>Added larger light variant, removed unecessary accessors. Fixed centered-movement bug! Added instructions!</t>
+  </si>
+  <si>
+    <t>Next Up: Menu shader, options menu, saving.</t>
   </si>
 </sst>
 </file>
@@ -221,8 +262,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0" tableBorderDxfId="6">
-  <autoFilter ref="A1:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="A1:C12"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Date" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="2" name="Hours" dataDxfId="3" totalsRowDxfId="2"/>
@@ -495,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +577,7 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(Table1[Hours])</f>
-        <v>24.5</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,7 +595,7 @@
       </c>
       <c r="F3" s="11">
         <f>COUNT(Table1[Date])</f>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -590,9 +631,75 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>42412</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>42428</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>42430</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>42431</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>42432</v>
+      </c>
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>42433</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Map Creator Setup / Fullscreen Toggle
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Cleaned up code, attempted to fix visiblity issues</t>
+  </si>
+  <si>
+    <t>Visibility now uses simplified segments, triangle issues?</t>
+  </si>
+  <si>
+    <t>Fullscreen toggling + UI refresh, level editor foundation / UI</t>
   </si>
 </sst>
 </file>
@@ -319,8 +325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0" tableBorderDxfId="6">
-  <autoFilter ref="A1:C16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C18" totalsRowShown="0" tableBorderDxfId="6">
+  <autoFilter ref="A1:C18"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Date" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="2" name="Hours" dataDxfId="3" totalsRowDxfId="2"/>
@@ -593,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +640,7 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(Table1[Hours])</f>
-        <v>52.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,7 +658,7 @@
       </c>
       <c r="F3" s="11">
         <f>COUNT(Table1[Date])</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -798,78 +804,100 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>42443</v>
+      </c>
+      <c r="B17" s="9">
+        <v>5</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>42447</v>
+      </c>
+      <c r="B18" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="3" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="3" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="3" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="3" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drei Setup / Broken Shadows Movement Fix
</commit_message>
<xml_diff>
--- a/Log.xlsx
+++ b/Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Plagman\Source\Repos\MonoGame\Broken Shadows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\GitHub\MonoGame\Broken Shadows\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -194,9 +194,6 @@
     <t xml:space="preserve">Revamped lighting to use visibility. </t>
   </si>
   <si>
-    <t>Next Up: Blurring, sounds, options menu, saving, enemies/lights,  disruptions, beatable level checks, flickering lights</t>
-  </si>
-  <si>
     <t>Cleaned up code, attempted to fix visiblity issues</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>Fullscreen toggling + UI refresh, level editor foundation / UI</t>
+  </si>
+  <si>
+    <t>Next Up: Light fix, sounds, options menu, saving, enemies/lights,  disruptions, beatable level checks, flickering lights</t>
   </si>
 </sst>
 </file>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +801,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,12 +823,12 @@
         <v>2.5</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>